<commit_message>
fixed mcq cleaning loophole
</commit_message>
<xml_diff>
--- a/survey_responses.xlsx
+++ b/survey_responses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGHS-PC\Documents\SIT stuff\trimester 1\python grp project\Data-Analysis-Project-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEon\Documents\GitHub\Data-Analysis-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E927AC5-B12E-4542-8D8B-FD24B30A0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F5D99C-8D67-40BA-A853-6EDC3EDF180D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="197">
   <si>
     <t>Gender</t>
   </si>
@@ -1114,27 +1114,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.69140625" customWidth="1"/>
+    <col min="2" max="2" width="17.23046875" customWidth="1"/>
+    <col min="3" max="3" width="18.84375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" customWidth="1"/>
-    <col min="11" max="11" width="42.109375" customWidth="1"/>
-    <col min="12" max="12" width="45.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.69140625" customWidth="1"/>
+    <col min="6" max="6" width="17.3046875" customWidth="1"/>
+    <col min="7" max="7" width="17.765625" customWidth="1"/>
+    <col min="8" max="8" width="18.23046875" customWidth="1"/>
+    <col min="9" max="9" width="21.3046875" customWidth="1"/>
+    <col min="10" max="10" width="22.84375" customWidth="1"/>
+    <col min="11" max="11" width="42.07421875" customWidth="1"/>
+    <col min="12" max="12" width="45.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="31.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
@@ -1214,14 +1214,14 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="9" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:13" s="9" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:13" s="9" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="9" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="9" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>88479</v>
       </c>
@@ -1275,21 +1275,9 @@
       <c r="E7">
         <v>1979</v>
       </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
       <c r="K7" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1288,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>48842</v>
       </c>
@@ -1338,7 +1326,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>36538</v>
       </c>
@@ -1376,7 +1364,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>88479</v>
       </c>
@@ -1414,7 +1402,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B11">
         <v>49985</v>
       </c>
@@ -1452,7 +1440,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>77840</v>
       </c>
@@ -1490,7 +1478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B13">
         <v>16125</v>
       </c>
@@ -1528,7 +1516,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>47054</v>
       </c>
@@ -1566,7 +1554,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B15">
         <v>33203</v>
       </c>
@@ -1604,7 +1592,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B16">
         <v>73779</v>
       </c>
@@ -1639,7 +1627,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>94580</v>
       </c>
@@ -1677,7 +1665,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B18">
         <v>32353</v>
       </c>
@@ -1715,7 +1703,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B19">
         <v>64594</v>
       </c>
@@ -1753,7 +1741,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B20">
         <v>27048</v>
       </c>
@@ -1791,7 +1779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B21">
         <v>30058</v>
       </c>
@@ -1829,7 +1817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B22">
         <v>90525</v>
       </c>
@@ -1867,7 +1855,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B23">
         <v>14960</v>
       </c>
@@ -1905,7 +1893,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B24">
         <v>78649</v>
       </c>
@@ -1943,7 +1931,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B25">
         <v>48411</v>
       </c>
@@ -1981,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B26">
         <v>54591</v>
       </c>
@@ -2019,7 +2007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B27">
         <v>72857</v>
       </c>
@@ -2057,7 +2045,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B28">
         <v>35019</v>
       </c>
@@ -2095,7 +2083,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B29">
         <v>37428</v>
       </c>
@@ -2133,7 +2121,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B30">
         <v>15277</v>
       </c>
@@ -2171,7 +2159,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B31">
         <v>29180</v>
       </c>
@@ -2209,7 +2197,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B32">
         <v>62592</v>
       </c>
@@ -2247,7 +2235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B33">
         <v>53755</v>
       </c>
@@ -2285,7 +2273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B34">
         <v>24641</v>
       </c>
@@ -2323,7 +2311,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B35">
         <v>98389</v>
       </c>
@@ -2361,7 +2349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B36">
         <v>54853</v>
       </c>
@@ -2399,7 +2387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B37">
         <v>19082</v>
       </c>
@@ -2437,7 +2425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B38">
         <v>65375</v>
       </c>
@@ -2475,7 +2463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B39">
         <v>49784</v>
       </c>
@@ -2513,7 +2501,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B40">
         <v>67129</v>
       </c>
@@ -2551,7 +2539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B41">
         <v>15370</v>
       </c>
@@ -2589,7 +2577,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B42">
         <v>88414</v>
       </c>
@@ -2627,7 +2615,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B43">
         <v>55454</v>
       </c>
@@ -2665,7 +2653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B44">
         <v>64745</v>
       </c>
@@ -2703,7 +2691,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B45">
         <v>82337</v>
       </c>
@@ -2741,7 +2729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B46">
         <v>83546</v>
       </c>
@@ -2779,7 +2767,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B47">
         <v>16925</v>
       </c>
@@ -2817,7 +2805,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B48">
         <v>53967</v>
       </c>
@@ -2855,7 +2843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B49">
         <v>10604</v>
       </c>
@@ -2893,7 +2881,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B50">
         <v>87980</v>
       </c>
@@ -2931,7 +2919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B51">
         <v>64170</v>
       </c>
@@ -2969,7 +2957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B52">
         <v>40435</v>
       </c>
@@ -3007,7 +2995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B53">
         <v>58090</v>
       </c>
@@ -3045,7 +3033,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B54">
         <v>79615</v>
       </c>
@@ -3083,7 +3071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B55">
         <v>90391</v>
       </c>
@@ -3121,7 +3109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B56">
         <v>72730</v>
       </c>
@@ -3156,7 +3144,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B57">
         <v>42596</v>
       </c>
@@ -3194,7 +3182,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B58">
         <v>33692</v>
       </c>
@@ -3232,7 +3220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B59">
         <v>49617</v>
       </c>
@@ -3270,7 +3258,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B60">
         <v>83823</v>
       </c>
@@ -3308,7 +3296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B61">
         <v>36875</v>
       </c>
@@ -3346,7 +3334,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B62">
         <v>22150</v>
       </c>
@@ -3384,7 +3372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B63">
         <v>78974</v>
       </c>
@@ -3422,7 +3410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B64">
         <v>54617</v>
       </c>
@@ -3460,7 +3448,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B65">
         <v>96327</v>
       </c>
@@ -3498,7 +3486,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B66">
         <v>98299</v>
       </c>
@@ -3536,7 +3524,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B67">
         <v>50399</v>
       </c>
@@ -3574,7 +3562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B68">
         <v>46881</v>
       </c>
@@ -3612,7 +3600,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B69">
         <v>18376</v>
       </c>
@@ -3650,7 +3638,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B70">
         <v>96281</v>
       </c>
@@ -3688,7 +3676,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B71">
         <v>72274</v>
       </c>
@@ -3726,7 +3714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B72">
         <v>34154</v>
       </c>
@@ -3764,7 +3752,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B73">
         <v>16187</v>
       </c>
@@ -3802,7 +3790,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B74">
         <v>30726</v>
       </c>
@@ -3840,7 +3828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B75">
         <v>13289</v>
       </c>
@@ -3878,7 +3866,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B76">
         <v>55161</v>
       </c>
@@ -3916,7 +3904,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B77">
         <v>16390</v>
       </c>
@@ -3954,7 +3942,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B78">
         <v>28354</v>
       </c>
@@ -3989,7 +3977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B79">
         <v>47144</v>
       </c>
@@ -4027,7 +4015,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B80">
         <v>32809</v>
       </c>
@@ -4065,7 +4053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B81">
         <v>58256</v>
       </c>
@@ -4103,7 +4091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B82">
         <v>56911</v>
       </c>
@@ -4141,7 +4129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B83">
         <v>26633</v>
       </c>
@@ -4179,7 +4167,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B84">
         <v>38538</v>
       </c>
@@ -4217,7 +4205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B85">
         <v>71208</v>
       </c>
@@ -4255,7 +4243,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B86">
         <v>66513</v>
       </c>
@@ -4293,7 +4281,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B87">
         <v>83630</v>
       </c>
@@ -4331,7 +4319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B88">
         <v>44038</v>
       </c>
@@ -4369,7 +4357,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B89">
         <v>69787</v>
       </c>
@@ -4407,7 +4395,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B90">
         <v>37079</v>
       </c>
@@ -4445,7 +4433,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B91">
         <v>29800</v>
       </c>
@@ -4483,7 +4471,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B92">
         <v>78328</v>
       </c>
@@ -4521,7 +4509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B93">
         <v>14582</v>
       </c>
@@ -4559,7 +4547,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B94">
         <v>93629</v>
       </c>
@@ -4597,7 +4585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B95">
         <v>14565</v>
       </c>
@@ -4635,7 +4623,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B96">
         <v>13595</v>
       </c>
@@ -4673,7 +4661,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B97">
         <v>75642</v>
       </c>
@@ -4711,7 +4699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B98">
         <v>52814</v>
       </c>
@@ -4749,7 +4737,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B99">
         <v>80357</v>
       </c>
@@ -4787,7 +4775,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B100">
         <v>58286</v>
       </c>
@@ -4825,7 +4813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B101">
         <v>95807</v>
       </c>
@@ -4863,7 +4851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B102">
         <v>74932</v>
       </c>
@@ -4901,7 +4889,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B103">
         <v>92469</v>
       </c>
@@ -4939,7 +4927,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B104">
         <v>86602</v>
       </c>
@@ -4977,7 +4965,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B105">
         <v>38229</v>
       </c>
@@ -5015,7 +5003,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B106">
         <v>43989</v>
       </c>
@@ -5053,7 +5041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B107">
         <v>43945</v>
       </c>
@@ -5091,7 +5079,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B108">
         <v>73143</v>
       </c>
@@ -5129,7 +5117,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B109">
         <v>73573</v>
       </c>
@@ -5167,7 +5155,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B110">
         <v>77406</v>
       </c>
@@ -5205,7 +5193,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B111">
         <v>56115</v>
       </c>
@@ -5243,7 +5231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B112">
         <v>82644</v>
       </c>
@@ -5281,7 +5269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B113">
         <v>54590</v>
       </c>
@@ -5319,7 +5307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B114">
         <v>77406</v>
       </c>
@@ -5357,7 +5345,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B115">
         <v>28056</v>
       </c>
@@ -5395,7 +5383,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B116">
         <v>74507</v>
       </c>
@@ -5433,7 +5421,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B117">
         <v>21645</v>
       </c>
@@ -5471,7 +5459,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B118">
         <v>82952</v>
       </c>
@@ -5509,7 +5497,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B119">
         <v>86304</v>
       </c>
@@ -5547,7 +5535,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B120">
         <v>81618</v>
       </c>
@@ -5585,7 +5573,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B121">
         <v>75141</v>
       </c>
@@ -5623,7 +5611,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B122">
         <v>53691</v>
       </c>
@@ -5661,7 +5649,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B123">
         <v>79908</v>
       </c>
@@ -5699,7 +5687,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B124">
         <v>74998</v>
       </c>
@@ -5737,7 +5725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B125">
         <v>78839</v>
       </c>
@@ -5775,7 +5763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B126">
         <v>22850</v>
       </c>
@@ -5813,7 +5801,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B127">
         <v>30987</v>
       </c>
@@ -5851,7 +5839,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B128">
         <v>60859</v>
       </c>
@@ -5889,7 +5877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B129">
         <v>50930</v>
       </c>
@@ -5927,7 +5915,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B130">
         <v>46812</v>
       </c>
@@ -5965,7 +5953,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B131">
         <v>35280</v>
       </c>
@@ -6003,7 +5991,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B132">
         <v>94878</v>
       </c>
@@ -6041,7 +6029,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B133">
         <v>83188</v>
       </c>
@@ -6079,7 +6067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B134">
         <v>76161</v>
       </c>
@@ -6117,7 +6105,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B135">
         <v>18344</v>
       </c>
@@ -6155,7 +6143,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B136">
         <v>35118</v>
       </c>
@@ -6193,7 +6181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B137">
         <v>20874</v>
       </c>
@@ -6231,7 +6219,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B138">
         <v>33306</v>
       </c>
@@ -6269,7 +6257,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="139" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B139">
         <v>65880</v>
       </c>
@@ -6307,7 +6295,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="140" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B140">
         <v>34716</v>
       </c>
@@ -6345,7 +6333,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B141">
         <v>60567</v>
       </c>
@@ -6383,7 +6371,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B142">
         <v>91701</v>
       </c>
@@ -6421,7 +6409,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B143">
         <v>64315</v>
       </c>
@@ -6459,7 +6447,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="144" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B144">
         <v>92533</v>
       </c>
@@ -6497,7 +6485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B145">
         <v>99745</v>
       </c>
@@ -6535,7 +6523,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="146" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B146">
         <v>65925</v>
       </c>
@@ -6573,7 +6561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B147">
         <v>25742</v>
       </c>
@@ -6611,7 +6599,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B148">
         <v>78835</v>
       </c>
@@ -6649,7 +6637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="149" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B149">
         <v>73336</v>
       </c>
@@ -6687,7 +6675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="150" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B150">
         <v>12019</v>
       </c>
@@ -6725,7 +6713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B151">
         <v>92008</v>
       </c>
@@ -6763,7 +6751,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B152">
         <v>19273</v>
       </c>
@@ -6801,7 +6789,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B153">
         <v>85557</v>
       </c>
@@ -6839,7 +6827,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B154">
         <v>49700</v>
       </c>
@@ -6877,7 +6865,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B155">
         <v>54880</v>
       </c>
@@ -6915,7 +6903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B156">
         <v>55426</v>
       </c>
@@ -6953,7 +6941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="157" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B157">
         <v>30844</v>
       </c>
@@ -6991,7 +6979,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B158">
         <v>53619</v>
       </c>
@@ -7029,7 +7017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="159" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B159">
         <v>33543</v>
       </c>
@@ -7067,7 +7055,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="160" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B160">
         <v>70231</v>
       </c>
@@ -7105,7 +7093,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="161" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B161">
         <v>75324</v>
       </c>
@@ -7143,7 +7131,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="162" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B162">
         <v>97761</v>
       </c>
@@ -7181,7 +7169,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="163" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B163">
         <v>57083</v>
       </c>
@@ -7219,7 +7207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="164" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B164">
         <v>93416</v>
       </c>
@@ -7257,7 +7245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="165" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B165">
         <v>98652</v>
       </c>
@@ -7295,7 +7283,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="166" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B166">
         <v>62998</v>
       </c>
@@ -7330,7 +7318,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="167" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B167">
         <v>65940</v>
       </c>
@@ -7368,7 +7356,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="168" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B168">
         <v>29642</v>
       </c>
@@ -7406,7 +7394,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="169" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B169">
         <v>18852</v>
       </c>
@@ -7444,7 +7432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="170" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B170">
         <v>77620</v>
       </c>
@@ -7482,7 +7470,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="171" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B171">
         <v>93189</v>
       </c>
@@ -7520,7 +7508,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B172">
         <v>27489</v>
       </c>
@@ -7558,7 +7546,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="173" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B173">
         <v>34135</v>
       </c>
@@ -7596,7 +7584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="174" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B174">
         <v>11638</v>
       </c>
@@ -7634,7 +7622,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B175">
         <v>30411</v>
       </c>
@@ -7672,7 +7660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B176">
         <v>10924</v>
       </c>
@@ -7710,7 +7698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B177">
         <v>25694</v>
       </c>
@@ -7748,7 +7736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B178">
         <v>77985</v>
       </c>
@@ -7786,7 +7774,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B179">
         <v>39729</v>
       </c>
@@ -7824,7 +7812,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="180" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B180">
         <v>37837</v>
       </c>
@@ -7862,7 +7850,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B181">
         <v>22557</v>
       </c>
@@ -7900,7 +7888,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B182">
         <v>22104</v>
       </c>
@@ -7938,7 +7926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="183" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B183">
         <v>47923</v>
       </c>
@@ -7976,7 +7964,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="184" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B184">
         <v>97312</v>
       </c>
@@ -8014,7 +8002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="185" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B185">
         <v>30795</v>
       </c>
@@ -8052,7 +8040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="186" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B186">
         <v>90837</v>
       </c>
@@ -8090,7 +8078,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="187" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B187">
         <v>22282</v>
       </c>
@@ -8128,7 +8116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B188">
         <v>53045</v>
       </c>
@@ -8166,7 +8154,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="189" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B189">
         <v>97312</v>
       </c>
@@ -8204,7 +8192,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="190" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B190">
         <v>58068</v>
       </c>
@@ -8242,7 +8230,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="191" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B191">
         <v>78812</v>
       </c>
@@ -8280,7 +8268,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B192">
         <v>25640</v>
       </c>
@@ -8318,7 +8306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B193">
         <v>75105</v>
       </c>
@@ -8356,7 +8344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B194">
         <v>10322</v>
       </c>
@@ -8394,7 +8382,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="195" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B195">
         <v>95811</v>
       </c>
@@ -8432,7 +8420,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="196" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B196">
         <v>48693</v>
       </c>
@@ -8470,7 +8458,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B197">
         <v>27938</v>
       </c>
@@ -8508,7 +8496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B198">
         <v>26192</v>
       </c>
@@ -8546,7 +8534,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="199" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B199">
         <v>31717</v>
       </c>
@@ -8584,7 +8572,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B200">
         <v>52112</v>
       </c>
@@ -8622,7 +8610,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="201" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B201">
         <v>98035</v>
       </c>
@@ -8660,7 +8648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B202">
         <v>93302</v>
       </c>
@@ -8698,7 +8686,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="203" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B203">
         <v>34110</v>
       </c>
@@ -8736,7 +8724,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="204" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B204">
         <v>11109</v>
       </c>
@@ -8774,7 +8762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="205" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B205">
         <v>33346</v>
       </c>

</xml_diff>